<commit_message>
Fixed handling of missing target_ids
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27716"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\ITR\ITR-tool\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFD4959-2F0D-40CA-9677-F573F6591675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F67917A-CBE9-4716-BF45-1A6E9410D02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35685" yWindow="4005" windowWidth="27120" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30375" yWindow="2925" windowWidth="27120" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -1214,8 +1214,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:U120" totalsRowShown="0">
-  <autoFilter ref="A1:U120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:U138" totalsRowShown="0">
+  <autoFilter ref="A1:U138" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
@@ -3701,7 +3701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I111" workbookViewId="0">
       <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIxed t_score + updated dependencies
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter.nystrom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\ITR\ITR-tool\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2062CF2F-FB1F-4C41-B33E-714C033CB71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4306F42-FB2E-4957-85A2-EC0C0A5DA0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="75" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="323">
   <si>
     <t>company_name</t>
   </si>
@@ -729,9 +729,6 @@
     <t>T57</t>
   </si>
   <si>
-    <t>T58</t>
-  </si>
-  <si>
     <t>T59</t>
   </si>
   <si>
@@ -1006,6 +1003,9 @@
   </si>
   <si>
     <t>T135</t>
+  </si>
+  <si>
+    <t>T_TS3</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:U118" totalsRowShown="0">
-  <autoFilter ref="A1:U118" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <autoFilter ref="A1:U118" xr:uid="{00000000-0009-0000-0100-000002000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="T_score"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
@@ -1491,10 +1497,10 @@
         <v>1</v>
       </c>
       <c r="K1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" t="s">
         <v>283</v>
-      </c>
-      <c r="L1" t="s">
-        <v>284</v>
       </c>
       <c r="M1" t="s">
         <v>152</v>
@@ -1515,49 +1521,49 @@
         <v>164</v>
       </c>
       <c r="S1" t="s">
+        <v>285</v>
+      </c>
+      <c r="T1" t="s">
         <v>286</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>287</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>288</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>289</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>290</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>291</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>292</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>293</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>294</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>295</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>296</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>297</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>298</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>299</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -3636,7 +3642,7 @@
   <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3669,16 +3675,16 @@
         <v>155</v>
       </c>
       <c r="E1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" t="s">
         <v>301</v>
-      </c>
-      <c r="F1" t="s">
-        <v>302</v>
       </c>
       <c r="G1" t="s">
         <v>156</v>
       </c>
       <c r="H1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I1" t="s">
         <v>157</v>
@@ -3702,7 +3708,7 @@
         <v>128</v>
       </c>
       <c r="P1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q1" t="s">
         <v>160</v>
@@ -3720,7 +3726,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" hidden="1">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>131</v>
       </c>
       <c r="H2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -3770,7 +3776,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" hidden="1">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -3787,7 +3793,7 @@
         <v>133</v>
       </c>
       <c r="H3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -3823,7 +3829,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" hidden="1">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" hidden="1">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" hidden="1">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" hidden="1">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>131</v>
       </c>
       <c r="H7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -4038,7 +4044,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" hidden="1">
       <c r="A8" t="s">
         <v>170</v>
       </c>
@@ -4085,7 +4091,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" hidden="1">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -4102,7 +4108,7 @@
         <v>131</v>
       </c>
       <c r="H9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -4138,7 +4144,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" hidden="1">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -4155,7 +4161,7 @@
         <v>131</v>
       </c>
       <c r="H10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -4191,7 +4197,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" hidden="1">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -4208,7 +4214,7 @@
         <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -4244,7 +4250,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" hidden="1">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>131</v>
       </c>
       <c r="H12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -4294,7 +4300,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" hidden="1">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -4308,7 +4314,7 @@
         <v>131</v>
       </c>
       <c r="H13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -4344,7 +4350,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" hidden="1">
       <c r="A14" t="s">
         <v>177</v>
       </c>
@@ -4358,7 +4364,7 @@
         <v>131</v>
       </c>
       <c r="H14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -4394,7 +4400,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" hidden="1">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -4408,7 +4414,7 @@
         <v>131</v>
       </c>
       <c r="H15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -4444,7 +4450,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" hidden="1">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>131</v>
       </c>
       <c r="H16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -4494,7 +4500,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" hidden="1">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -4541,7 +4547,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" hidden="1">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" hidden="1">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -4635,7 +4641,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" hidden="1">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -4682,7 +4688,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" hidden="1">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" hidden="1">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4776,7 +4782,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" hidden="1">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -4826,7 +4832,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" hidden="1">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -4840,7 +4846,7 @@
         <v>131</v>
       </c>
       <c r="H24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -4876,7 +4882,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" hidden="1">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -4893,7 +4899,7 @@
         <v>131</v>
       </c>
       <c r="H25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I25">
         <v>0.95</v>
@@ -4929,7 +4935,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" hidden="1">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" hidden="1">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -5023,7 +5029,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" hidden="1">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -5037,7 +5043,7 @@
         <v>131</v>
       </c>
       <c r="H28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I28">
         <v>0.99</v>
@@ -5073,7 +5079,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" hidden="1">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5123,7 +5129,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" hidden="1">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -5170,7 +5176,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" hidden="1">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -5184,7 +5190,7 @@
         <v>131</v>
       </c>
       <c r="H31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -5220,7 +5226,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" hidden="1">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -5270,7 +5276,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" hidden="1">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -5320,7 +5326,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" hidden="1">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -5334,7 +5340,7 @@
         <v>133</v>
       </c>
       <c r="H34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -5367,7 +5373,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" hidden="1">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5384,7 +5390,7 @@
         <v>131</v>
       </c>
       <c r="H35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I35">
         <v>0.71</v>
@@ -5414,7 +5420,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" hidden="1">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -5431,7 +5437,7 @@
         <v>131</v>
       </c>
       <c r="H36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I36">
         <v>0.75</v>
@@ -5467,7 +5473,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" hidden="1">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -5481,7 +5487,7 @@
         <v>131</v>
       </c>
       <c r="H37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -5517,7 +5523,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" hidden="1">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -5531,7 +5537,7 @@
         <v>131</v>
       </c>
       <c r="H38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I38">
         <v>0.86</v>
@@ -5567,7 +5573,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" hidden="1">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -5581,7 +5587,7 @@
         <v>131</v>
       </c>
       <c r="H39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I39">
         <v>0.86</v>
@@ -5617,7 +5623,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" hidden="1">
       <c r="A40" t="s">
         <v>170</v>
       </c>
@@ -5634,7 +5640,7 @@
         <v>131</v>
       </c>
       <c r="H40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I40">
         <v>0.65</v>
@@ -5673,7 +5679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" hidden="1">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -5687,7 +5693,7 @@
         <v>131</v>
       </c>
       <c r="H41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -5723,7 +5729,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" hidden="1">
       <c r="A42" t="s">
         <v>172</v>
       </c>
@@ -5740,7 +5746,7 @@
         <v>133</v>
       </c>
       <c r="H42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -5773,7 +5779,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" hidden="1">
       <c r="A43" t="s">
         <v>173</v>
       </c>
@@ -5790,7 +5796,7 @@
         <v>131</v>
       </c>
       <c r="H43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -5826,7 +5832,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" hidden="1">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -5840,7 +5846,7 @@
         <v>131</v>
       </c>
       <c r="H44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I44">
         <v>0.7</v>
@@ -5876,7 +5882,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" hidden="1">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -5890,7 +5896,7 @@
         <v>131</v>
       </c>
       <c r="H45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -5926,7 +5932,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" hidden="1">
       <c r="A46" t="s">
         <v>176</v>
       </c>
@@ -5940,7 +5946,7 @@
         <v>131</v>
       </c>
       <c r="H46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -5976,7 +5982,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" hidden="1">
       <c r="A47" t="s">
         <v>177</v>
       </c>
@@ -5990,7 +5996,7 @@
         <v>131</v>
       </c>
       <c r="H47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I47">
         <v>0.97</v>
@@ -6026,7 +6032,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" hidden="1">
       <c r="A48" t="s">
         <v>178</v>
       </c>
@@ -6040,7 +6046,7 @@
         <v>131</v>
       </c>
       <c r="H48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -6084,7 +6090,7 @@
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E49">
         <v>3.13</v>
@@ -6093,10 +6099,10 @@
         <v>2.19</v>
       </c>
       <c r="G49" t="s">
-        <v>131</v>
-      </c>
-      <c r="H49" t="s">
-        <v>304</v>
+        <v>142</v>
+      </c>
+      <c r="H49">
+        <v>15</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -6129,10 +6135,10 @@
         <v>0.24</v>
       </c>
       <c r="U49" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" hidden="1">
       <c r="A50" t="s">
         <v>181</v>
       </c>
@@ -6149,7 +6155,7 @@
         <v>131</v>
       </c>
       <c r="H50" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I50">
         <v>0.75</v>
@@ -6182,10 +6188,10 @@
         <v>0.7</v>
       </c>
       <c r="U50" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" hidden="1">
       <c r="A51" t="s">
         <v>81</v>
       </c>
@@ -6202,7 +6208,7 @@
         <v>131</v>
       </c>
       <c r="H51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I51">
         <v>1</v>
@@ -6235,10 +6241,10 @@
         <v>0.7</v>
       </c>
       <c r="U51" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" hidden="1">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -6252,7 +6258,7 @@
         <v>131</v>
       </c>
       <c r="H52" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I52">
         <v>1</v>
@@ -6285,10 +6291,10 @@
         <v>0</v>
       </c>
       <c r="U52" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" hidden="1">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -6302,7 +6308,7 @@
         <v>131</v>
       </c>
       <c r="H53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -6335,10 +6341,10 @@
         <v>0.6</v>
       </c>
       <c r="U53" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" hidden="1">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -6352,7 +6358,7 @@
         <v>131</v>
       </c>
       <c r="H54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I54">
         <v>0.95</v>
@@ -6385,10 +6391,10 @@
         <v>0.7</v>
       </c>
       <c r="U54" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" hidden="1">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -6405,7 +6411,7 @@
         <v>131</v>
       </c>
       <c r="H55" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I55">
         <v>0.95</v>
@@ -6438,10 +6444,10 @@
         <v>0.47789999999999999</v>
       </c>
       <c r="U55" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" hidden="1">
       <c r="A56" t="s">
         <v>81</v>
       </c>
@@ -6458,7 +6464,7 @@
         <v>131</v>
       </c>
       <c r="H56" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I56">
         <v>0.93</v>
@@ -6491,10 +6497,10 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="U56" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" hidden="1">
       <c r="A57" t="s">
         <v>83</v>
       </c>
@@ -6508,7 +6514,7 @@
         <v>131</v>
       </c>
       <c r="H57" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -6541,10 +6547,10 @@
         <v>0.79</v>
       </c>
       <c r="U57" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" hidden="1">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -6561,7 +6567,7 @@
         <v>131</v>
       </c>
       <c r="H58" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -6594,10 +6600,10 @@
         <v>0.7</v>
       </c>
       <c r="U58" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" hidden="1">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -6611,7 +6617,7 @@
         <v>139</v>
       </c>
       <c r="H59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -6641,10 +6647,10 @@
         <v>0</v>
       </c>
       <c r="U59" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" hidden="1">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -6661,7 +6667,7 @@
         <v>131</v>
       </c>
       <c r="H60" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -6694,10 +6700,10 @@
         <v>6.4100000000000004E-2</v>
       </c>
       <c r="U60" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" hidden="1">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -6744,10 +6750,10 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="U61" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" hidden="1">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -6761,7 +6767,7 @@
         <v>131</v>
       </c>
       <c r="H62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -6794,10 +6800,10 @@
         <v>0.11220000000000001</v>
       </c>
       <c r="U62" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" hidden="1">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -6814,7 +6820,7 @@
         <v>131</v>
       </c>
       <c r="H63" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I63">
         <v>1</v>
@@ -6847,10 +6853,10 @@
         <v>0.22870000000000001</v>
       </c>
       <c r="U63" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" hidden="1">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -6864,7 +6870,7 @@
         <v>131</v>
       </c>
       <c r="H64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I64">
         <v>1</v>
@@ -6897,10 +6903,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="U64" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" hidden="1">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -6917,7 +6923,7 @@
         <v>131</v>
       </c>
       <c r="H65" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -6950,10 +6956,10 @@
         <v>0.34</v>
       </c>
       <c r="U65" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" hidden="1">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -6970,7 +6976,7 @@
         <v>131</v>
       </c>
       <c r="H66" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -7003,10 +7009,10 @@
         <v>0.34</v>
       </c>
       <c r="U66" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" hidden="1">
       <c r="A67" t="s">
         <v>121</v>
       </c>
@@ -7050,10 +7056,10 @@
         <v>0.84400000000000008</v>
       </c>
       <c r="U67" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" hidden="1">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -7106,10 +7112,10 @@
         <v>0.85299999999999998</v>
       </c>
       <c r="U68" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" hidden="1">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -7126,7 +7132,7 @@
         <v>131</v>
       </c>
       <c r="H69" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -7159,10 +7165,10 @@
         <v>0.55670000000000008</v>
       </c>
       <c r="U69" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" hidden="1">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -7209,10 +7215,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U70" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" hidden="1">
       <c r="A71" t="s">
         <v>168</v>
       </c>
@@ -7259,10 +7265,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U71" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" hidden="1">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -7309,10 +7315,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U72" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" hidden="1">
       <c r="A73" t="s">
         <v>172</v>
       </c>
@@ -7329,7 +7335,7 @@
         <v>131</v>
       </c>
       <c r="H73" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I73">
         <v>0.93100000000000005</v>
@@ -7362,10 +7368,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U73" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" hidden="1">
       <c r="A74" t="s">
         <v>175</v>
       </c>
@@ -7382,7 +7388,7 @@
         <v>133</v>
       </c>
       <c r="H74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J74">
         <v>0.7</v>
@@ -7412,10 +7418,10 @@
         <v>0.93</v>
       </c>
       <c r="U74" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" hidden="1">
       <c r="A75" t="s">
         <v>177</v>
       </c>
@@ -7429,7 +7435,7 @@
         <v>139</v>
       </c>
       <c r="H75" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -7459,10 +7465,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U75" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" hidden="1">
       <c r="A76" t="s">
         <v>177</v>
       </c>
@@ -7476,7 +7482,7 @@
         <v>133</v>
       </c>
       <c r="H76" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -7506,10 +7512,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U76" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" hidden="1">
       <c r="A77" t="s">
         <v>178</v>
       </c>
@@ -7523,7 +7529,7 @@
         <v>139</v>
       </c>
       <c r="H77" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I77">
         <v>1</v>
@@ -7553,10 +7559,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U77" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" hidden="1">
       <c r="A78" t="s">
         <v>181</v>
       </c>
@@ -7570,7 +7576,7 @@
         <v>131</v>
       </c>
       <c r="H78" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I78">
         <v>1</v>
@@ -7603,10 +7609,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U78" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" hidden="1">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -7620,7 +7626,7 @@
         <v>131</v>
       </c>
       <c r="H79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I79">
         <v>1</v>
@@ -7653,10 +7659,10 @@
         <v>0</v>
       </c>
       <c r="U79" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" hidden="1">
       <c r="A80" t="s">
         <v>165</v>
       </c>
@@ -7673,7 +7679,7 @@
         <v>131</v>
       </c>
       <c r="H80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -7706,10 +7712,10 @@
         <v>0</v>
       </c>
       <c r="U80" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" hidden="1">
       <c r="A81" t="s">
         <v>166</v>
       </c>
@@ -7726,7 +7732,7 @@
         <v>131</v>
       </c>
       <c r="H81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I81">
         <v>1</v>
@@ -7759,10 +7765,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U81" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" hidden="1">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -7776,7 +7782,7 @@
         <v>139</v>
       </c>
       <c r="H82" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I82">
         <v>1</v>
@@ -7806,10 +7812,10 @@
         <v>0.33</v>
       </c>
       <c r="U82" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" hidden="1">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -7823,7 +7829,7 @@
         <v>133</v>
       </c>
       <c r="H83" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J83">
         <v>1</v>
@@ -7853,10 +7859,10 @@
         <v>0.82000000000000006</v>
       </c>
       <c r="U83" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" hidden="1">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -7873,7 +7879,7 @@
         <v>131</v>
       </c>
       <c r="H84" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I84">
         <v>0.87</v>
@@ -7906,10 +7912,10 @@
         <v>0.67</v>
       </c>
       <c r="U84" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" hidden="1">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -7953,10 +7959,10 @@
         <v>0.67</v>
       </c>
       <c r="U85" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" hidden="1">
       <c r="A86" t="s">
         <v>171</v>
       </c>
@@ -7970,7 +7976,7 @@
         <v>131</v>
       </c>
       <c r="H86" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I86">
         <v>0.27</v>
@@ -8003,10 +8009,10 @@
         <v>0.67</v>
       </c>
       <c r="U86" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" hidden="1">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -8023,7 +8029,7 @@
         <v>131</v>
       </c>
       <c r="H87" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I87">
         <v>1</v>
@@ -8056,10 +8062,10 @@
         <v>0</v>
       </c>
       <c r="U87" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="88" spans="1:21">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" hidden="1">
       <c r="A88" t="s">
         <v>173</v>
       </c>
@@ -8076,7 +8082,7 @@
         <v>131</v>
       </c>
       <c r="H88" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I88">
         <v>1</v>
@@ -8109,10 +8115,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U88" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" hidden="1">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -8159,10 +8165,10 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="U89" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" hidden="1">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -8179,7 +8185,7 @@
         <v>131</v>
       </c>
       <c r="H90" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I90">
         <v>1</v>
@@ -8212,10 +8218,10 @@
         <v>0.61</v>
       </c>
       <c r="U90" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" hidden="1">
       <c r="A91" t="s">
         <v>176</v>
       </c>
@@ -8229,7 +8235,7 @@
         <v>131</v>
       </c>
       <c r="H91" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I91">
         <v>0.94</v>
@@ -8262,10 +8268,10 @@
         <v>0.69000000000000006</v>
       </c>
       <c r="U91" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" hidden="1">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -8279,7 +8285,7 @@
         <v>131</v>
       </c>
       <c r="H92" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I92">
         <v>0.94</v>
@@ -8312,10 +8318,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="U92" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" hidden="1">
       <c r="A93" t="s">
         <v>178</v>
       </c>
@@ -8332,7 +8338,7 @@
         <v>131</v>
       </c>
       <c r="H93" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I93">
         <v>0.94</v>
@@ -8365,10 +8371,10 @@
         <v>0.57020000000000004</v>
       </c>
       <c r="U93" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="94" spans="1:21">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" hidden="1">
       <c r="A94" t="s">
         <v>179</v>
       </c>
@@ -8415,10 +8421,10 @@
         <v>0.67</v>
       </c>
       <c r="U94" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="95" spans="1:21">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" hidden="1">
       <c r="A95" t="s">
         <v>181</v>
       </c>
@@ -8435,7 +8441,7 @@
         <v>139</v>
       </c>
       <c r="H95" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I95">
         <v>0.99</v>
@@ -8465,10 +8471,10 @@
         <v>0.88300000000000001</v>
       </c>
       <c r="U95" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="96" spans="1:21">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" hidden="1">
       <c r="A96" t="s">
         <v>83</v>
       </c>
@@ -8482,7 +8488,7 @@
         <v>131</v>
       </c>
       <c r="H96" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I96">
         <v>1</v>
@@ -8515,10 +8521,10 @@
         <v>1</v>
       </c>
       <c r="U96" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="97" spans="1:21">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" hidden="1">
       <c r="A97" t="s">
         <v>85</v>
       </c>
@@ -8565,10 +8571,10 @@
         <v>1</v>
       </c>
       <c r="U97" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" hidden="1">
       <c r="A98" t="s">
         <v>81</v>
       </c>
@@ -8582,7 +8588,7 @@
         <v>131</v>
       </c>
       <c r="H98" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I98">
         <v>0.66839999999999999</v>
@@ -8615,10 +8621,10 @@
         <v>0.25</v>
       </c>
       <c r="U98" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="99" spans="1:21">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" hidden="1">
       <c r="A99" t="s">
         <v>83</v>
       </c>
@@ -8635,7 +8641,7 @@
         <v>131</v>
       </c>
       <c r="H99" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I99">
         <v>0.2024</v>
@@ -8668,10 +8674,10 @@
         <v>0.154</v>
       </c>
       <c r="U99" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" hidden="1">
       <c r="A100" t="s">
         <v>83</v>
       </c>
@@ -8688,7 +8694,7 @@
         <v>131</v>
       </c>
       <c r="H100" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I100">
         <v>0.66900000000000004</v>
@@ -8721,10 +8727,10 @@
         <v>0</v>
       </c>
       <c r="U100" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="101" spans="1:21">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" hidden="1">
       <c r="A101" t="s">
         <v>121</v>
       </c>
@@ -8738,7 +8744,7 @@
         <v>131</v>
       </c>
       <c r="H101" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I101">
         <v>0.5</v>
@@ -8774,10 +8780,10 @@
         <v>0</v>
       </c>
       <c r="U101" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="102" spans="1:21">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" hidden="1">
       <c r="A102" t="s">
         <v>121</v>
       </c>
@@ -8827,10 +8833,10 @@
         <v>0</v>
       </c>
       <c r="U102" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" hidden="1">
       <c r="A103" t="s">
         <v>121</v>
       </c>
@@ -8874,10 +8880,10 @@
         <v>0</v>
       </c>
       <c r="U103" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" hidden="1">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -8921,10 +8927,10 @@
         <v>0</v>
       </c>
       <c r="U104" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="105" spans="1:21">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" hidden="1">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -8968,10 +8974,10 @@
         <v>0</v>
       </c>
       <c r="U105" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" hidden="1">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -9015,10 +9021,10 @@
         <v>0</v>
       </c>
       <c r="U106" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" hidden="1">
       <c r="A107" t="s">
         <v>165</v>
       </c>
@@ -9065,10 +9071,10 @@
         <v>0.5</v>
       </c>
       <c r="U107" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="108" spans="1:21">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" hidden="1">
       <c r="A108" t="s">
         <v>165</v>
       </c>
@@ -9115,10 +9121,10 @@
         <v>0</v>
       </c>
       <c r="U108" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" hidden="1">
       <c r="A109" t="s">
         <v>165</v>
       </c>
@@ -9168,10 +9174,10 @@
         <v>0.85299999999999998</v>
       </c>
       <c r="U109" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" hidden="1">
       <c r="A110" t="s">
         <v>165</v>
       </c>
@@ -9218,10 +9224,10 @@
         <v>0</v>
       </c>
       <c r="U110" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" hidden="1">
       <c r="A111" t="s">
         <v>166</v>
       </c>
@@ -9265,10 +9271,10 @@
         <v>0.5</v>
       </c>
       <c r="U111" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" hidden="1">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -9315,10 +9321,10 @@
         <v>0.86</v>
       </c>
       <c r="U112" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" hidden="1">
       <c r="A113" t="s">
         <v>166</v>
       </c>
@@ -9365,10 +9371,10 @@
         <v>0.55670000000000008</v>
       </c>
       <c r="U113" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="114" spans="1:21">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" hidden="1">
       <c r="A114" t="s">
         <v>166</v>
       </c>
@@ -9415,7 +9421,7 @@
         <v>0</v>
       </c>
       <c r="U114" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:21">
@@ -9426,7 +9432,7 @@
         <v>8</v>
       </c>
       <c r="C115" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E115">
         <v>3.19</v>
@@ -9435,10 +9441,10 @@
         <v>2.17</v>
       </c>
       <c r="G115" t="s">
-        <v>131</v>
-      </c>
-      <c r="H115" t="s">
-        <v>304</v>
+        <v>142</v>
+      </c>
+      <c r="H115">
+        <v>15</v>
       </c>
       <c r="I115">
         <v>0</v>
@@ -9474,10 +9480,10 @@
         <v>0</v>
       </c>
       <c r="U115" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" hidden="1">
       <c r="A116" t="s">
         <v>166</v>
       </c>
@@ -9524,10 +9530,10 @@
         <v>0.55670000000000008</v>
       </c>
       <c r="U116" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="117" spans="1:21">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" hidden="1">
       <c r="A117" t="s">
         <v>166</v>
       </c>
@@ -9574,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="U117" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:21">
@@ -9585,7 +9591,7 @@
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E118">
         <v>2.8</v>
@@ -9594,10 +9600,10 @@
         <v>1.9</v>
       </c>
       <c r="G118" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H118">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="M118">
         <v>2018</v>
@@ -9621,7 +9627,7 @@
         <v>0</v>
       </c>
       <c r="U118" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>